<commit_message>
Fixed TSLint errors as per the latest ruleset
</commit_message>
<xml_diff>
--- a/documents/Published/KPIColumn/KPIColumnByMAQSoftwareChecklist.xlsx
+++ b/documents/Published/KPIColumn/KPIColumnByMAQSoftwareChecklist.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MAQUser\source\repos\NewRepo2\documents\Published\KPIColumn\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Custom Visual\documents\Published\KPIColumn\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D76F0D6A-DE0D-4847-A6E6-9911F948D069}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4448A4D6-5F61-4756-81A1-D4E885F44D52}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CFA628E8-139E-4A70-BE7A-AA996D28E374}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="125">
   <si>
     <t>S no</t>
   </si>
@@ -516,6 +516,21 @@
   </si>
   <si>
     <t>1. On right click of the chart and selecting the drillthrough option from the context-menu , the report will drillthrough to the newly created report page.</t>
+  </si>
+  <si>
+    <t>Internet Explorer</t>
+  </si>
+  <si>
+    <t>Edge</t>
+  </si>
+  <si>
+    <t>Chrome</t>
+  </si>
+  <si>
+    <t>Desktop</t>
+  </si>
+  <si>
+    <t>Pass</t>
   </si>
 </sst>
 </file>
@@ -677,7 +692,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -740,6 +755,9 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -755,6 +773,3091 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>5448300</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>2397559</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6A522481-334E-4DF2-B840-9EE6FA3EA398}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16916400" y="190500"/>
+          <a:ext cx="5448300" cy="2397559"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>7154265</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>2705464</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8AE3C78C-4181-4E23-9E19-1B9863B56661}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15525750" y="285750"/>
+          <a:ext cx="7097115" cy="2610214"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>386243</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>5076825</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>1962151</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{313531A7-C807-4452-829C-50AFCF671C35}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14306550" y="576743"/>
+          <a:ext cx="4972050" cy="1575908"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>457200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>5438775</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>2033108</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9B9A97D7-A71F-445F-ACE3-E90F7855F939}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13573125" y="647700"/>
+          <a:ext cx="4972050" cy="1575908"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>19051</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>162662</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>2552700</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8958159F-6882-4F32-A17E-FCC5F3670987}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="32908876" y="3152775"/>
+          <a:ext cx="5677636" cy="2476500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>5915025</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>2182551</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9383731D-2F1C-4AA9-9183-56A7D0239C3F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="25669875" y="3076576"/>
+          <a:ext cx="5915025" cy="2182550"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>5756551</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>2124075</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B4A4FE1B-774D-4FEA-B591-9C4C5D178C04}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13106400" y="3076575"/>
+          <a:ext cx="5756551" cy="2124075"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>52042</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>2219325</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A295B61D-3532-4D35-9F97-B2DC5228DCFE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="19707225" y="3076575"/>
+          <a:ext cx="6014692" cy="2219325"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>581026</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>304801</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>5438776</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>2084691</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{95A1C6BB-60DB-41F0-ABA7-D901F5DA8D45}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13687426" y="6705601"/>
+          <a:ext cx="4857750" cy="1779890"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>5200650</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>2003034</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{70629932-BF9B-4F0F-B18C-A472D30CB12D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="19831050" y="6543675"/>
+          <a:ext cx="5076825" cy="1860159"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>66676</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>6134100</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>2094354</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Picture 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1F671512-14C9-46F8-BE93-6E0EAA870060}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="26269950" y="6467476"/>
+          <a:ext cx="5534025" cy="2027678"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>4667250</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>2026074</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F1DB5C52-69E0-4503-9FBD-F3AAB1A11F2F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="33127950" y="6467475"/>
+          <a:ext cx="4429125" cy="1959399"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>266700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>5926982</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>2314575</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Picture 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DAC5D8FC-D6D3-4AE1-B9CE-42F140075402}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13325475" y="9077325"/>
+          <a:ext cx="5707907" cy="2047875"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>5707907</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>2047875</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Picture 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A1753AF6-5989-4857-AEAA-5B20E0EA1BB0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="19707225" y="8810625"/>
+          <a:ext cx="5707907" cy="2047875"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>285750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>6146057</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>2333625</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="Picture 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{635ECF31-C1E8-4EE0-817E-338E50C5F00A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="26108025" y="9096375"/>
+          <a:ext cx="5707907" cy="2047875"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>5456989</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>1704975</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="18" name="Picture 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{69F5D08B-6AAC-4983-8441-AFBC230E4090}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13106400" y="12344400"/>
+          <a:ext cx="5456989" cy="1704975"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>3514725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>5095875</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>8188</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="19" name="Picture 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8158F3FE-418C-4109-954D-8F09B3B13754}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="32946975" y="12325350"/>
+          <a:ext cx="5038725" cy="2208463"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>200026</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>5286375</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>2248200</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="20" name="Picture 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F6CF36F6-5123-41D1-9ECF-186ED8938BED}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="33499425" y="9010651"/>
+          <a:ext cx="4676775" cy="2048174"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>5456989</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>1704975</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="21" name="Picture 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1A9E728F-49B3-4CAD-BAE4-8FAAE692F5BC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="19707225" y="12344400"/>
+          <a:ext cx="5456989" cy="1704975"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>5456989</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>1704975</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="22" name="Picture 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{14A8BA46-FD89-4955-8D63-100C00B3582A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="25669875" y="12344400"/>
+          <a:ext cx="5456989" cy="1704975"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>5114925</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>2105324</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="23" name="Picture 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CDED873C-F6F3-4E81-97C8-7FD40EFFCBE1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="33327975" y="14582775"/>
+          <a:ext cx="4676775" cy="2048174"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>5707907</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>2047875</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="25" name="Picture 24">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5B580493-9283-4FD8-A2CD-43416DFC5BD1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="25669875" y="14525625"/>
+          <a:ext cx="5707907" cy="2047875"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>5898407</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>2076450</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="26" name="Picture 25">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DBC841AA-6D12-4B92-B6AE-C9B6FDBF61BD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="19650075" y="14554200"/>
+          <a:ext cx="5707907" cy="2047875"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>5707907</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>2047875</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="27" name="Picture 26">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{81114EBC-D20D-4012-9361-C7D1B0EE9EE9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13106400" y="14525625"/>
+          <a:ext cx="5707907" cy="2047875"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>5162550</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>2195337</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="28" name="Picture 27">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EF5DB1D6-1774-4290-8BB2-1B420CD192AF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="32937450" y="16735425"/>
+          <a:ext cx="4867275" cy="2176287"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>676275</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>66676</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>6405266</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>1876426</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="29" name="Picture 28">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{01B32145-B149-4426-82EB-048EFE7D47C1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="26098500" y="16783051"/>
+          <a:ext cx="5728991" cy="1809750"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>5578228</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>1762125</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="30" name="Picture 29">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{38E3001B-AF34-4CE1-9ACA-044C7896EFB2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="19459575" y="16716375"/>
+          <a:ext cx="5578228" cy="1762125"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>247651</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>5490985</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>1943101</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="31" name="Picture 30">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B5766830-04C7-45E3-BE20-2750239CD39E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13230225" y="16964026"/>
+          <a:ext cx="5367160" cy="1695450"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>5019675</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>40638</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="32" name="Picture 31">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C7DC0A3F-4503-4DF7-BDB9-7B14225BBBEA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13106400" y="18945225"/>
+          <a:ext cx="5019675" cy="1564638"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>5019675</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>40638</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="33" name="Picture 32">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{656F3E36-CAF4-45F4-9876-AE218BE56423}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="19459575" y="18945225"/>
+          <a:ext cx="5019675" cy="1564638"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>5019675</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>40638</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="34" name="Picture 33">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B24BF362-33D8-493B-9FC1-47DEBD329454}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="25422225" y="18945225"/>
+          <a:ext cx="5019675" cy="1564638"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>695325</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>2209800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>4152900</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>1522519</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="35" name="Picture 34">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B7E7673E-E49D-4A07-8A3E-3BC93517F183}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="33337500" y="18926175"/>
+          <a:ext cx="3457575" cy="1541569"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>590550</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>5457825</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>2155188</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="38" name="Picture 37">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F4F0CB27-04B5-4566-8C92-762117010915}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13544550" y="21059775"/>
+          <a:ext cx="5019675" cy="1564638"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>542925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>5353050</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>2107563</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="39" name="Picture 38">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BB203783-971F-4C19-B454-1A00DAA9AFF2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="19792950" y="21012150"/>
+          <a:ext cx="5019675" cy="1564638"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>514350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>5467350</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>2078988</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="40" name="Picture 39">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{85CCC638-8029-445D-B136-9B5B89764DB4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="25869900" y="20983575"/>
+          <a:ext cx="5019675" cy="1564638"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>733425</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>419100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>4191000</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>1960669</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="41" name="Picture 40">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4AA8C95D-A500-4D85-B8FA-73652FECAC04}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="33375600" y="20888325"/>
+          <a:ext cx="3457575" cy="1541569"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>2771775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>5037942</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>2171700</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="42" name="Picture 41">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{55D6A612-FD6B-4598-8FA5-A3F17470D87E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="32785050" y="23241000"/>
+          <a:ext cx="4895067" cy="2219325"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>5235275</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>1428750</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="43" name="Picture 42">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7CDCCA66-7AF7-445D-AFFD-5F3851E65642}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13106401" y="23288625"/>
+          <a:ext cx="5235274" cy="1428750"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>5235274</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>1428750</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="44" name="Picture 43">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0D4DAA72-5E1B-44CC-AF61-10F33C3C75AD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="19459575" y="23288625"/>
+          <a:ext cx="5235274" cy="1428750"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1266825</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>361950</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>6502099</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>1790700</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="45" name="Picture 44">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7AAABD7F-310D-4A74-B1DC-B90EE73B47AE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="26689050" y="23650575"/>
+          <a:ext cx="5235274" cy="1428750"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>123826</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>352425</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>6219826</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>3624001</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="46" name="Picture 45">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{23BD32EE-6C84-4CF1-8E17-236C3D045F0A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13230226" y="26317575"/>
+          <a:ext cx="6096000" cy="3271576"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>3271576</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="47" name="Picture 46">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{91CB0C7C-F21D-4522-B2DD-99D275FACDA8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="19459575" y="25965150"/>
+          <a:ext cx="6096000" cy="3271576"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>6096000</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>3271576</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="48" name="Picture 47">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9CAFD6DF-9592-4B5C-874C-017E245D170A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="25422225" y="25965150"/>
+          <a:ext cx="6096000" cy="3271576"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>4238625</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>3614253</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="49" name="Picture 48">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{32FA1A41-5156-409C-9134-72BDA9C8D297}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId19"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="32642175" y="25965150"/>
+          <a:ext cx="4238625" cy="3614253"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>5191125</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>1410576</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="50" name="Picture 49">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D5A44A82-2670-4A69-998A-F53DE51D4A8C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId20"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13106400" y="30222825"/>
+          <a:ext cx="5191125" cy="1410576"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>5372100</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>1459752</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="51" name="Picture 50">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D14EA169-25A4-416C-800B-C4C6CD7A59AF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId20"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="19459575" y="30222825"/>
+          <a:ext cx="5372100" cy="1459752"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>5629275</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>1529633</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="52" name="Picture 51">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B0C123D6-9DA1-4593-A4EA-105266F4B99B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId20"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="25422225" y="30222825"/>
+          <a:ext cx="5629275" cy="1529633"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>4457701</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>1989859</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="53" name="Picture 52">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EE723DB0-8A74-4C65-B44F-9CC7AF942784}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId21"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="32642176" y="30222825"/>
+          <a:ext cx="4457700" cy="1989859"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>4752975</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>2142960</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="54" name="Picture 53">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2686C80F-1B76-4E01-A347-DE0F0FC1C4FC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId22"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="32642175" y="32556450"/>
+          <a:ext cx="4752975" cy="2142960"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>5555035</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>1504950</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="55" name="Picture 54">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{627D1D4B-CB44-45E7-81A9-F391A0776194}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId23"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13106400" y="32556450"/>
+          <a:ext cx="5555035" cy="1504950"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>4922183</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>1333500</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="56" name="Picture 55">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4A612587-2D37-4197-818B-AA1EAC700715}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId23"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="19459575" y="32556450"/>
+          <a:ext cx="4922183" cy="1333500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>6840630</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>1933575</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="57" name="Picture 56">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{50875C33-31BF-4B31-A296-C0A1AE8BD196}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId23"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="25793700" y="32737425"/>
+          <a:ext cx="6469155" cy="1752600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>57151</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>4124325</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>1843363</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="58" name="Picture 57">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6E60BD76-EFBC-4FDD-9150-37752E42198F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId24"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="32718375" y="35252026"/>
+          <a:ext cx="4048125" cy="1786212"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>466726</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>5687516</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="59" name="Picture 58">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4ABC8550-C6ED-4558-890A-41C947900979}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId25"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13573126" y="35223450"/>
+          <a:ext cx="5220790" cy="1914525"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>161926</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>4905376</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>1834729</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="60" name="Picture 59">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{52370C12-CFC0-4D25-8A2A-9AD40EEBF84C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId25"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="19621501" y="35290125"/>
+          <a:ext cx="4743450" cy="1739479"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>876300</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>76201</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>5857875</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>1903003</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="61" name="Picture 60">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{612D3FFC-8726-4385-B8FF-8FC8213AED79}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId25"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="26298525" y="35271076"/>
+          <a:ext cx="4981575" cy="1826802"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>419100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>5782765</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>2333625</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="62" name="Picture 61">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A72DCECC-28EB-4D8E-BDFA-A203F9A6BD3F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId25"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13668375" y="37528500"/>
+          <a:ext cx="5220790" cy="1914525"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>5220790</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>1914525</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="63" name="Picture 62">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3341D940-14A3-43C3-8D37-B8F06279B848}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId25"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="19459575" y="37109400"/>
+          <a:ext cx="5220790" cy="1914525"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>5220790</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>1914525</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="64" name="Picture 63">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{292AF087-7007-46DF-80D0-091616D286DA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId25"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="25422225" y="37109400"/>
+          <a:ext cx="5220790" cy="1914525"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>4048125</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>1786212</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="65" name="Picture 64">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A748212B-C952-41C5-B9AB-A6C860C1D38B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId24"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="32642175" y="37109400"/>
+          <a:ext cx="4048125" cy="1786212"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>4795061</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>2190751</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="66" name="Picture 65">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E272DC0F-A407-4480-9310-23A2793FD4E7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId26"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="32642176" y="39776401"/>
+          <a:ext cx="4795060" cy="2190750"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1047750</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>219075</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>6486525</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>2262291</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="67" name="Picture 66">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B4230E96-7E7A-42FC-917F-2528AE9D97CE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId27"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="26469975" y="39995475"/>
+          <a:ext cx="5438775" cy="2043216"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>361949</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>5858858</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>2217455</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="68" name="Picture 67">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A2200B72-933F-4137-B7FD-E2627EFE29E1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId27"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="19821524" y="39928800"/>
+          <a:ext cx="5496909" cy="2065055"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>5819706</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>2152650</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="69" name="Picture 68">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5A006E17-60A7-4C80-B2C4-84FC6EE0BA03}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId27"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13601700" y="39928800"/>
+          <a:ext cx="5324406" cy="2000250"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>4876800</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>1799608</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="73" name="Picture 72">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2D03027F-16B3-4F17-9F36-5F64BEA1D7E3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId28"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="32642175" y="42462450"/>
+          <a:ext cx="4876800" cy="1799608"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>4019550</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>1466850</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="74" name="Picture 73">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A0DDFF7D-2E58-47BB-AC14-BA5DAD66FF75}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId29"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13106400" y="42462450"/>
+          <a:ext cx="4019550" cy="1466850"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>3448050</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>1762336</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="75" name="Picture 74">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4DB0DFD5-F35F-4696-AE8F-29366BA06B3A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId29"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="19459575" y="42462450"/>
+          <a:ext cx="3448050" cy="1762336"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>4019550</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>1466850</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="76" name="Picture 75">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C8570AFC-027F-4630-B448-1EB2AF9BED37}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId29"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="25422225" y="42462450"/>
+          <a:ext cx="4019550" cy="1466850"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>85724</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>95249</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>4857750</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>38400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="71" name="Picture 70">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CF759C42-2B2B-43D9-9353-F06564EB1CEF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId30"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13192124" y="44472224"/>
+          <a:ext cx="4772026" cy="3105451"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>95249</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>76201</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>4838700</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>2759789</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="24" name="Picture 23">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{51F2B714-1BC9-403B-A174-390AD3A604CC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId31"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="19554824" y="44453176"/>
+          <a:ext cx="4743451" cy="2683588"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1054,10 +4157,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95C560CE-405B-4CA8-AB3A-A0EEBCD256B2}">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1066,9 +4169,13 @@
     <col min="3" max="3" width="42.7109375" customWidth="1"/>
     <col min="4" max="4" width="48.140625" customWidth="1"/>
     <col min="5" max="5" width="68.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="95.28515625" customWidth="1"/>
+    <col min="7" max="7" width="89.42578125" customWidth="1"/>
+    <col min="8" max="8" width="108.28515625" customWidth="1"/>
+    <col min="9" max="9" width="83" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1084,8 +4191,20 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="F1" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="227.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1101,8 +4220,9 @@
       <c r="E2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="H2" s="1"/>
+    </row>
+    <row r="3" spans="1:9" ht="261.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1119,7 +4239,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="189.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>11</v>
       </c>
@@ -1130,7 +4250,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="278.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1147,7 +4267,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="171.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1164,7 +4284,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="172.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>10</v>
       </c>
@@ -1175,7 +4295,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="175.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>5</v>
       </c>
@@ -1192,7 +4312,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1209,7 +4329,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="222" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1226,7 +4346,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="210.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1243,7 +4363,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="305.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1260,7 +4380,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1276,8 +4396,20 @@
       <c r="E13" s="2" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" ht="116.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F13" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="183.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1294,7 +4426,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="207.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1311,7 +4443,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="150.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1328,7 +4460,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="210" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1345,7 +4477,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="211.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1362,7 +4494,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="150.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1379,26 +4511,27 @@
         <v>112</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="249" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
         <v>116</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C20" s="22" t="s">
         <v>117</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="D20" s="22" t="s">
         <v>118</v>
       </c>
-      <c r="E20" s="2" t="s">
+      <c r="E20" s="22" t="s">
         <v>119</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>